<commit_message>
adding colors to first row in excel output
</commit_message>
<xml_diff>
--- a/data/DataGeneration_5_24.xlsx
+++ b/data/DataGeneration_5_24.xlsx
@@ -29,7 +29,7 @@
       <name val="David"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="13">
     <fill>
       <patternFill/>
     </fill>
@@ -46,6 +46,60 @@
       <patternFill patternType="solid">
         <fgColor rgb="00D3EAD3"/>
         <bgColor rgb="00D3EAD3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00A2C4C9"/>
+        <bgColor rgb="00A2C4C9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F4CCCC"/>
+        <bgColor rgb="00F4CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D3D3D3"/>
+        <bgColor rgb="00D3D3D3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F9CB9C"/>
+        <bgColor rgb="00F9CB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D9EAD3"/>
+        <bgColor rgb="00D9EAD3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF2CC"/>
+        <bgColor rgb="00FFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="009FC5E8"/>
+        <bgColor rgb="009FC5E8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0093C47D"/>
+        <bgColor rgb="0093C47D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00EAD1DC"/>
+        <bgColor rgb="00EAD1DC"/>
       </patternFill>
     </fill>
   </fills>
@@ -67,9 +121,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
@@ -437,7 +500,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BF14"/>
+  <dimension ref="A1:BG14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,526 +519,532 @@
       <c r="H1" s="1" t="n"/>
       <c r="I1" s="1" t="n"/>
       <c r="J1" s="1" t="n"/>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="n"/>
+      <c r="L1" s="2" t="inlineStr">
         <is>
           <t>B10/20 - AgPlenus</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="2" t="inlineStr">
         <is>
           <t>B10/20 - AgPlenus.1</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="2" t="inlineStr">
         <is>
           <t>B10/20 - AgPlenus.2</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="2" t="inlineStr">
         <is>
           <t>B10/20 - AgPlenus.3</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="2" t="inlineStr">
         <is>
           <t>B10/20 - AgPlenus.4</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="2" t="inlineStr">
         <is>
           <t>B10/20 - AgPlenus.5</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="3" t="inlineStr">
         <is>
           <t>B20/20 - Lavie- Bio</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="3" t="inlineStr">
         <is>
           <t>B20/20 - Lavie- Bio.1</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="3" t="inlineStr">
         <is>
           <t>B20/20 - Lavie- Bio.2</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="3" t="inlineStr">
         <is>
           <t>B20/20 - Lavie- Bio.3</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="3" t="inlineStr">
         <is>
           <t>B20/20 - Lavie- Bio.4</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="4" t="inlineStr">
         <is>
           <t>B20/20 - Lavie- Bio.5</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="4" t="inlineStr">
         <is>
           <t>B20/20 - Lavie- Bio.6</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="4" t="inlineStr">
         <is>
           <t>B20/20 - Lavie- Bio.7</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="4" t="inlineStr">
         <is>
           <t>B20/20 - Lavie- Bio.8</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="5" t="inlineStr">
         <is>
           <t>B40/20 - CPB</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="5" t="inlineStr">
         <is>
           <t>B40/20 - CPB.1</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="5" t="inlineStr">
         <is>
           <t>B40/20 - CPB.2</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="5" t="inlineStr">
         <is>
           <t>B40/20 - CPB.3</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="6" t="inlineStr">
         <is>
           <t>B70/20 - Biomica</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="6" t="inlineStr">
         <is>
           <t>B70/20 - Biomica.1</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="6" t="inlineStr">
         <is>
           <t>B70/20 - Biomica.2</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="6" t="inlineStr">
         <is>
           <t>B70/20 - Biomica.3</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="6" t="inlineStr">
         <is>
           <t>B70/20 - Biomica.4</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="6" t="inlineStr">
         <is>
           <t>B74/20 - Canonic</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="7" t="inlineStr">
         <is>
           <t>B74/20 - Canonic.1</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="7" t="inlineStr">
         <is>
           <t>B74/20 - Canonic.2</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="7" t="inlineStr">
         <is>
           <t>B74/20 - Canonic.3</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="7" t="inlineStr">
         <is>
           <t>B74/20 - Canonic.4</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="7" t="inlineStr">
         <is>
           <t>B74/20 - Canonic.5</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="8" t="inlineStr">
         <is>
           <t>B80/20 - PRoduct</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="8" t="inlineStr">
         <is>
           <t>B80/20 - PRoduct.1</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="8" t="inlineStr">
         <is>
           <t>B80/20 - PRoduct.2</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="8" t="inlineStr">
         <is>
           <t>B80/20 - PRoduct.3</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="8" t="inlineStr">
         <is>
           <t>B80/20 - PRoduct.4</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="8" t="inlineStr">
         <is>
           <t>B80/20 - PRoduct.5</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="8" t="inlineStr">
         <is>
           <t>B80/20 - PRoduct.6</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AW1" s="8" t="inlineStr">
         <is>
           <t>B80/20 - PRoduct.7</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AX1" s="8" t="inlineStr">
         <is>
           <t>B80/20 - PRoduct.8</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AY1" s="8" t="inlineStr">
         <is>
           <t>B80/20 - PRoduct.9</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AZ1" s="9" t="inlineStr">
         <is>
           <t>B72/20 - Casterra</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BA1" s="9" t="inlineStr">
         <is>
           <t>B72/20 - Casterra.1</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BB1" s="9" t="inlineStr">
         <is>
           <t>B72/20 - Casterra.2</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BC1" s="9" t="inlineStr">
         <is>
           <t>B72/20 - Casterra.3</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BD1" s="9" t="inlineStr">
         <is>
           <t>B72/20 - Casterra.4</t>
         </is>
       </c>
-      <c r="BD1" s="1" t="inlineStr">
+      <c r="BE1" s="9" t="inlineStr">
         <is>
           <t>B72/20 - Casterra.5</t>
         </is>
       </c>
-      <c r="BE1" s="1" t="n"/>
-      <c r="BF1" s="1" t="n"/>
+      <c r="BF1" s="10" t="n"/>
+      <c r="BG1" s="10" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="11" t="inlineStr">
         <is>
           <t>Entry Type</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="11" t="inlineStr">
         <is>
           <t>Employee ID</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="11" t="inlineStr">
         <is>
           <t>Exp Type</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="D2" s="11" t="inlineStr">
         <is>
           <t>Role Ending</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="E2" s="11" t="inlineStr">
+        <is>
+          <t>Department</t>
+        </is>
+      </c>
+      <c r="F2" s="11" t="inlineStr">
         <is>
           <t>Jira name</t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="G2" s="11" t="inlineStr">
         <is>
           <t>Employee Name</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
+      <c r="H2" s="11" t="inlineStr">
         <is>
           <t>Approved by</t>
         </is>
       </c>
-      <c r="H2" s="2" t="inlineStr">
+      <c r="I2" s="11" t="inlineStr">
         <is>
           <t>Month</t>
         </is>
       </c>
-      <c r="I2" s="2" t="inlineStr">
+      <c r="J2" s="11" t="inlineStr">
         <is>
           <t>FTE Contract</t>
         </is>
       </c>
-      <c r="J2" s="2" t="inlineStr">
+      <c r="K2" s="11" t="inlineStr">
         <is>
           <t>FTE left to Assign</t>
         </is>
       </c>
-      <c r="K2" s="2" t="inlineStr">
+      <c r="L2" s="11" t="inlineStr">
         <is>
           <t>P21 - agPlenus Tech</t>
         </is>
       </c>
-      <c r="L2" s="2" t="inlineStr">
+      <c r="M2" s="11" t="inlineStr">
         <is>
           <t>P210 - Herbicides Corteva</t>
         </is>
       </c>
-      <c r="M2" s="2" t="inlineStr">
+      <c r="N2" s="11" t="inlineStr">
         <is>
           <t>P33 - Insectecide</t>
         </is>
       </c>
-      <c r="N2" s="2" t="inlineStr">
+      <c r="O2" s="11" t="inlineStr">
         <is>
           <t>P211 - Herbicides APTH1</t>
         </is>
       </c>
-      <c r="O2" s="2" t="inlineStr">
+      <c r="P2" s="11" t="inlineStr">
         <is>
           <t>P23 - Herbicides</t>
         </is>
       </c>
-      <c r="P2" s="2" t="inlineStr">
+      <c r="Q2" s="11" t="inlineStr">
         <is>
           <t>P24 - Fungicides</t>
         </is>
       </c>
-      <c r="Q2" s="2" t="inlineStr">
+      <c r="R2" s="11" t="inlineStr">
         <is>
           <t>P145 - Corteva</t>
         </is>
       </c>
-      <c r="R2" s="2" t="inlineStr">
+      <c r="S2" s="11" t="inlineStr">
         <is>
           <t>P192 - LAV 321</t>
         </is>
       </c>
-      <c r="S2" s="2" t="inlineStr">
+      <c r="T2" s="11" t="inlineStr">
         <is>
           <t>P19 - Yalos</t>
         </is>
       </c>
-      <c r="T2" s="2" t="inlineStr">
+      <c r="U2" s="11" t="inlineStr">
         <is>
           <t>P84 - New program</t>
         </is>
       </c>
-      <c r="U2" s="2" t="inlineStr">
+      <c r="V2" s="11" t="inlineStr">
         <is>
           <t>P82 - ICL</t>
         </is>
       </c>
-      <c r="V2" s="2" t="inlineStr">
+      <c r="W2" s="11" t="inlineStr">
         <is>
           <t>P86 - Product</t>
         </is>
       </c>
-      <c r="W2" s="2" t="inlineStr">
+      <c r="X2" s="11" t="inlineStr">
         <is>
           <t>P85 - Syngenta</t>
         </is>
       </c>
-      <c r="X2" s="2" t="inlineStr">
+      <c r="Y2" s="11" t="inlineStr">
         <is>
           <t>P87 - LAV311</t>
         </is>
       </c>
-      <c r="Y2" s="2" t="inlineStr">
+      <c r="Z2" s="11" t="inlineStr">
         <is>
           <t>P999 - General</t>
         </is>
       </c>
-      <c r="Z2" s="2" t="inlineStr">
+      <c r="AA2" s="11" t="inlineStr">
         <is>
           <t>P271 - CPB Upkeep Computational</t>
         </is>
       </c>
-      <c r="AA2" s="2" t="inlineStr">
+      <c r="AB2" s="11" t="inlineStr">
         <is>
           <t>P279 - CPB projects Computational</t>
         </is>
       </c>
-      <c r="AB2" s="2" t="inlineStr">
+      <c r="AC2" s="11" t="inlineStr">
         <is>
           <t>P275 - CPB Upkeep Experimental</t>
         </is>
       </c>
-      <c r="AC2" s="2" t="inlineStr">
+      <c r="AD2" s="11" t="inlineStr">
         <is>
           <t>P281 - CPB projects Experimental</t>
         </is>
       </c>
-      <c r="AD2" s="2" t="inlineStr">
+      <c r="AE2" s="11" t="inlineStr">
         <is>
           <t>P250 - TcdAB2</t>
         </is>
       </c>
-      <c r="AE2" s="2" t="inlineStr">
+      <c r="AF2" s="11" t="inlineStr">
         <is>
           <t>P251 - MRSA 50S2</t>
         </is>
       </c>
-      <c r="AF2" s="2" t="inlineStr">
+      <c r="AG2" s="11" t="inlineStr">
         <is>
           <t>P252 - Cancer Immun adjuvant2</t>
         </is>
       </c>
-      <c r="AG2" s="2" t="inlineStr">
+      <c r="AH2" s="11" t="inlineStr">
         <is>
           <t>P258 - New Indication TBD</t>
         </is>
       </c>
-      <c r="AH2" s="2" t="inlineStr">
+      <c r="AI2" s="11" t="inlineStr">
         <is>
           <t>P999 - General4</t>
         </is>
       </c>
-      <c r="AI2" s="2" t="inlineStr">
+      <c r="AJ2" s="11" t="inlineStr">
         <is>
           <t>P197 - Breeding general</t>
         </is>
       </c>
-      <c r="AJ2" s="2" t="inlineStr">
+      <c r="AK2" s="11" t="inlineStr">
         <is>
           <t>P205 - Product development</t>
         </is>
       </c>
-      <c r="AK2" s="2" t="inlineStr">
+      <c r="AL2" s="11" t="inlineStr">
         <is>
           <t>P209 - Computational Dev</t>
         </is>
       </c>
-      <c r="AL2" s="2" t="inlineStr">
+      <c r="AM2" s="11" t="inlineStr">
         <is>
           <t>P212 - Propagation general</t>
         </is>
       </c>
-      <c r="AM2" s="2" t="inlineStr">
+      <c r="AN2" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">P213 - Breeding general </t>
         </is>
       </c>
-      <c r="AN2" s="2" t="inlineStr">
+      <c r="AO2" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">P216 - Core collection &amp; Data base </t>
         </is>
       </c>
-      <c r="AO2" s="2" t="inlineStr">
+      <c r="AP2" s="11" t="inlineStr">
         <is>
           <t>P290 - Colors</t>
         </is>
       </c>
-      <c r="AP2" s="2" t="inlineStr">
+      <c r="AQ2" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">P273 - Product- Upkeep MB </t>
         </is>
       </c>
-      <c r="AQ2" s="2" t="inlineStr">
+      <c r="AR2" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">P274 - Product- Upkeep CP </t>
         </is>
       </c>
-      <c r="AR2" s="2" t="inlineStr">
+      <c r="AS2" s="11" t="inlineStr">
         <is>
           <t>P272 - Product- Upkeep GR</t>
         </is>
       </c>
-      <c r="AS2" s="2" t="inlineStr">
+      <c r="AT2" s="11" t="inlineStr">
         <is>
           <t>P264 -Product CP</t>
         </is>
       </c>
-      <c r="AT2" s="2" t="inlineStr">
+      <c r="AU2" s="11" t="inlineStr">
         <is>
           <t>P258 - Rafael</t>
         </is>
       </c>
-      <c r="AU2" s="2" t="inlineStr">
+      <c r="AV2" s="11" t="inlineStr">
         <is>
           <t>P265 - Product- MB</t>
         </is>
       </c>
-      <c r="AV2" s="2" t="inlineStr">
+      <c r="AW2" s="11" t="inlineStr">
         <is>
           <t>P282 - Product general</t>
         </is>
       </c>
-      <c r="AW2" s="2" t="inlineStr">
+      <c r="AX2" s="11" t="inlineStr">
         <is>
           <t>P400 - Corp4clima</t>
         </is>
       </c>
-      <c r="AX2" s="2" t="inlineStr">
+      <c r="AY2" s="11" t="inlineStr">
         <is>
           <t>P401 - The Kitchen</t>
         </is>
       </c>
-      <c r="AY2" s="2" t="inlineStr">
+      <c r="AZ2" s="11" t="inlineStr">
         <is>
           <t>P401 - Casterra DB &amp; LIMS</t>
         </is>
       </c>
-      <c r="AZ2" s="2" t="inlineStr">
+      <c r="BA2" s="11" t="inlineStr">
         <is>
           <t>P402 - Casterra Generator</t>
         </is>
       </c>
-      <c r="BA2" s="2" t="inlineStr">
+      <c r="BB2" s="11" t="inlineStr">
         <is>
           <t>P403 - Casterra RUN Generator</t>
         </is>
       </c>
-      <c r="BB2" s="2" t="inlineStr">
+      <c r="BC2" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">P404 - Casterra Developing new varieties </t>
         </is>
       </c>
-      <c r="BC2" s="2" t="inlineStr">
+      <c r="BD2" s="11" t="inlineStr">
         <is>
           <t>P405 - Casterra Develop no RICIN lines</t>
         </is>
       </c>
-      <c r="BD2" s="2" t="inlineStr">
+      <c r="BE2" s="11" t="inlineStr">
         <is>
           <t>P999 - General2</t>
         </is>
       </c>
-      <c r="BE2" s="2" t="inlineStr">
+      <c r="BF2" s="11" t="inlineStr">
         <is>
           <t>OH</t>
         </is>
       </c>
-      <c r="BF2" s="2" t="inlineStr">
+      <c r="BG2" s="11" t="inlineStr">
         <is>
           <t>P0 - Vacation / Sickness</t>
         </is>
@@ -987,34 +1056,36 @@
           <t>Budget</t>
         </is>
       </c>
-      <c r="B3" s="3" t="n"/>
-      <c r="C3" s="3" t="n"/>
-      <c r="D3" s="3" t="inlineStr">
+      <c r="B3" s="12" t="n"/>
+      <c r="C3" s="12" t="n"/>
+      <c r="D3" s="12" t="inlineStr">
         <is>
           <t>T104 - Data Gathering</t>
         </is>
       </c>
-      <c r="E3" s="3" t="n"/>
-      <c r="F3" s="3" t="inlineStr">
+      <c r="E3" s="12" t="inlineStr">
+        <is>
+          <t>411 - Data Generation</t>
+        </is>
+      </c>
+      <c r="F3" s="12" t="n"/>
+      <c r="G3" s="12" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="G3" s="3" t="n"/>
-      <c r="H3" s="3" t="inlineStr">
+      <c r="H3" s="12" t="n"/>
+      <c r="I3" s="12" t="inlineStr">
         <is>
           <t>2024-01</t>
         </is>
       </c>
-      <c r="I3" s="3" t="n">
+      <c r="J3" s="12" t="n">
         <v>69</v>
       </c>
-      <c r="J3" s="3" t="n">
+      <c r="K3" s="12" t="n">
         <v>69</v>
       </c>
-      <c r="K3" s="1" t="n">
-        <v/>
-      </c>
       <c r="L3" s="1" t="n">
         <v/>
       </c>
@@ -1154,6 +1225,9 @@
         <v/>
       </c>
       <c r="BF3" s="1" t="n">
+        <v/>
+      </c>
+      <c r="BG3" s="1" t="n">
         <v/>
       </c>
     </row>
@@ -1163,34 +1237,36 @@
           <t>Budget</t>
         </is>
       </c>
-      <c r="B4" s="3" t="n"/>
-      <c r="C4" s="3" t="n"/>
-      <c r="D4" s="3" t="inlineStr">
+      <c r="B4" s="12" t="n"/>
+      <c r="C4" s="12" t="n"/>
+      <c r="D4" s="12" t="inlineStr">
         <is>
           <t>T104 - Data Gathering</t>
         </is>
       </c>
-      <c r="E4" s="3" t="n"/>
-      <c r="F4" s="3" t="inlineStr">
+      <c r="E4" s="12" t="inlineStr">
+        <is>
+          <t>411 - Data Generation</t>
+        </is>
+      </c>
+      <c r="F4" s="12" t="n"/>
+      <c r="G4" s="12" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="G4" s="3" t="n"/>
-      <c r="H4" s="3" t="inlineStr">
+      <c r="H4" s="12" t="n"/>
+      <c r="I4" s="12" t="inlineStr">
         <is>
           <t>2024-02</t>
         </is>
       </c>
-      <c r="I4" s="3" t="n">
+      <c r="J4" s="12" t="n">
         <v>60</v>
       </c>
-      <c r="J4" s="3" t="n">
+      <c r="K4" s="12" t="n">
         <v>60</v>
       </c>
-      <c r="K4" s="1" t="n">
-        <v/>
-      </c>
       <c r="L4" s="1" t="n">
         <v/>
       </c>
@@ -1330,6 +1406,9 @@
         <v/>
       </c>
       <c r="BF4" s="1" t="n">
+        <v/>
+      </c>
+      <c r="BG4" s="1" t="n">
         <v/>
       </c>
     </row>
@@ -1339,37 +1418,39 @@
           <t>Budget</t>
         </is>
       </c>
-      <c r="B5" s="3" t="n"/>
-      <c r="C5" s="3" t="n"/>
-      <c r="D5" s="3" t="inlineStr">
+      <c r="B5" s="12" t="n"/>
+      <c r="C5" s="12" t="n"/>
+      <c r="D5" s="12" t="inlineStr">
         <is>
           <t>T104 - Data Gathering</t>
         </is>
       </c>
-      <c r="E5" s="3" t="n"/>
-      <c r="F5" s="3" t="inlineStr">
+      <c r="E5" s="12" t="inlineStr">
+        <is>
+          <t>411 - Data Generation</t>
+        </is>
+      </c>
+      <c r="F5" s="12" t="n"/>
+      <c r="G5" s="12" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="G5" s="3" t="n"/>
-      <c r="H5" s="3" t="inlineStr">
+      <c r="H5" s="12" t="n"/>
+      <c r="I5" s="12" t="inlineStr">
         <is>
           <t>2024-03</t>
         </is>
       </c>
-      <c r="I5" s="3" t="n">
+      <c r="J5" s="12" t="n">
         <v>63</v>
       </c>
-      <c r="J5" s="3" t="n">
+      <c r="K5" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="K5" s="1" t="n">
+      <c r="L5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="L5" s="1" t="n">
-        <v/>
-      </c>
       <c r="M5" s="1" t="n">
         <v/>
       </c>
@@ -1383,11 +1464,11 @@
         <v/>
       </c>
       <c r="Q5" s="1" t="n">
+        <v/>
+      </c>
+      <c r="R5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="R5" s="1" t="n">
-        <v/>
-      </c>
       <c r="S5" s="1" t="n">
         <v/>
       </c>
@@ -1395,11 +1476,11 @@
         <v/>
       </c>
       <c r="U5" s="1" t="n">
+        <v/>
+      </c>
+      <c r="V5" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="V5" s="1" t="n">
-        <v/>
-      </c>
       <c r="W5" s="1" t="n">
         <v/>
       </c>
@@ -1413,17 +1494,17 @@
         <v/>
       </c>
       <c r="AA5" s="1" t="n">
+        <v/>
+      </c>
+      <c r="AB5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="AB5" s="1" t="n">
-        <v/>
-      </c>
       <c r="AC5" s="1" t="n">
+        <v/>
+      </c>
+      <c r="AD5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="AD5" s="1" t="n">
-        <v/>
-      </c>
       <c r="AE5" s="1" t="n">
         <v/>
       </c>
@@ -1449,11 +1530,11 @@
         <v/>
       </c>
       <c r="AM5" s="1" t="n">
+        <v/>
+      </c>
+      <c r="AN5" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="AN5" s="1" t="n">
-        <v/>
-      </c>
       <c r="AO5" s="1" t="n">
         <v/>
       </c>
@@ -1479,11 +1560,11 @@
         <v/>
       </c>
       <c r="AW5" s="1" t="n">
+        <v/>
+      </c>
+      <c r="AX5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="AX5" s="1" t="n">
-        <v/>
-      </c>
       <c r="AY5" s="1" t="n">
         <v/>
       </c>
@@ -1494,18 +1575,21 @@
         <v/>
       </c>
       <c r="BB5" s="1" t="n">
+        <v/>
+      </c>
+      <c r="BC5" s="1" t="n">
         <v>6.8</v>
       </c>
-      <c r="BC5" s="1" t="n">
-        <v/>
-      </c>
       <c r="BD5" s="1" t="n">
         <v/>
       </c>
       <c r="BE5" s="1" t="n">
+        <v/>
+      </c>
+      <c r="BF5" s="1" t="n">
         <v>4.2</v>
       </c>
-      <c r="BF5" s="1" t="n">
+      <c r="BG5" s="1" t="n">
         <v>11</v>
       </c>
     </row>
@@ -1515,34 +1599,36 @@
           <t>Budget</t>
         </is>
       </c>
-      <c r="B6" s="3" t="n"/>
-      <c r="C6" s="3" t="n"/>
-      <c r="D6" s="3" t="inlineStr">
+      <c r="B6" s="12" t="n"/>
+      <c r="C6" s="12" t="n"/>
+      <c r="D6" s="12" t="inlineStr">
         <is>
           <t>T104 - Data Gathering</t>
         </is>
       </c>
-      <c r="E6" s="3" t="n"/>
-      <c r="F6" s="3" t="inlineStr">
+      <c r="E6" s="12" t="inlineStr">
+        <is>
+          <t>411 - Data Generation</t>
+        </is>
+      </c>
+      <c r="F6" s="12" t="n"/>
+      <c r="G6" s="12" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="G6" s="3" t="n"/>
-      <c r="H6" s="3" t="inlineStr">
+      <c r="H6" s="12" t="n"/>
+      <c r="I6" s="12" t="inlineStr">
         <is>
           <t>2024-04</t>
         </is>
       </c>
-      <c r="I6" s="3" t="n">
+      <c r="J6" s="12" t="n">
         <v>55.5</v>
       </c>
-      <c r="J6" s="3" t="n">
+      <c r="K6" s="12" t="n">
         <v>55.5</v>
       </c>
-      <c r="K6" s="1" t="n">
-        <v/>
-      </c>
       <c r="L6" s="1" t="n">
         <v/>
       </c>
@@ -1682,6 +1768,9 @@
         <v/>
       </c>
       <c r="BF6" s="1" t="n">
+        <v/>
+      </c>
+      <c r="BG6" s="1" t="n">
         <v/>
       </c>
     </row>
@@ -1691,34 +1780,36 @@
           <t>Budget</t>
         </is>
       </c>
-      <c r="B7" s="3" t="n"/>
-      <c r="C7" s="3" t="n"/>
-      <c r="D7" s="3" t="inlineStr">
+      <c r="B7" s="12" t="n"/>
+      <c r="C7" s="12" t="n"/>
+      <c r="D7" s="12" t="inlineStr">
         <is>
           <t>T104 - Data Gathering</t>
         </is>
       </c>
-      <c r="E7" s="3" t="n"/>
-      <c r="F7" s="3" t="inlineStr">
+      <c r="E7" s="12" t="inlineStr">
+        <is>
+          <t>411 - Data Generation</t>
+        </is>
+      </c>
+      <c r="F7" s="12" t="n"/>
+      <c r="G7" s="12" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="G7" s="3" t="n"/>
-      <c r="H7" s="3" t="inlineStr">
+      <c r="H7" s="12" t="n"/>
+      <c r="I7" s="12" t="inlineStr">
         <is>
           <t>2024-05</t>
         </is>
       </c>
-      <c r="I7" s="3" t="n">
+      <c r="J7" s="12" t="n">
         <v>61.5</v>
       </c>
-      <c r="J7" s="3" t="n">
+      <c r="K7" s="12" t="n">
         <v>61.5</v>
       </c>
-      <c r="K7" s="1" t="n">
-        <v/>
-      </c>
       <c r="L7" s="1" t="n">
         <v/>
       </c>
@@ -1858,6 +1949,9 @@
         <v/>
       </c>
       <c r="BF7" s="1" t="n">
+        <v/>
+      </c>
+      <c r="BG7" s="1" t="n">
         <v/>
       </c>
     </row>
@@ -1867,34 +1961,36 @@
           <t>Budget</t>
         </is>
       </c>
-      <c r="B8" s="3" t="n"/>
-      <c r="C8" s="3" t="n"/>
-      <c r="D8" s="3" t="inlineStr">
+      <c r="B8" s="12" t="n"/>
+      <c r="C8" s="12" t="n"/>
+      <c r="D8" s="12" t="inlineStr">
         <is>
           <t>T104 - Data Gathering</t>
         </is>
       </c>
-      <c r="E8" s="3" t="n"/>
-      <c r="F8" s="3" t="inlineStr">
+      <c r="E8" s="12" t="inlineStr">
+        <is>
+          <t>411 - Data Generation</t>
+        </is>
+      </c>
+      <c r="F8" s="12" t="n"/>
+      <c r="G8" s="12" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="G8" s="3" t="n"/>
-      <c r="H8" s="3" t="inlineStr">
+      <c r="H8" s="12" t="n"/>
+      <c r="I8" s="12" t="inlineStr">
         <is>
           <t>2024-06</t>
         </is>
       </c>
-      <c r="I8" s="3" t="n">
+      <c r="J8" s="12" t="n">
         <v>58.5</v>
       </c>
-      <c r="J8" s="3" t="n">
+      <c r="K8" s="12" t="n">
         <v>58.5</v>
       </c>
-      <c r="K8" s="1" t="n">
-        <v/>
-      </c>
       <c r="L8" s="1" t="n">
         <v/>
       </c>
@@ -2034,6 +2130,9 @@
         <v/>
       </c>
       <c r="BF8" s="1" t="n">
+        <v/>
+      </c>
+      <c r="BG8" s="1" t="n">
         <v/>
       </c>
     </row>
@@ -2043,34 +2142,36 @@
           <t>Budget</t>
         </is>
       </c>
-      <c r="B9" s="3" t="n"/>
-      <c r="C9" s="3" t="n"/>
-      <c r="D9" s="3" t="inlineStr">
+      <c r="B9" s="12" t="n"/>
+      <c r="C9" s="12" t="n"/>
+      <c r="D9" s="12" t="inlineStr">
         <is>
           <t>T104 - Data Gathering</t>
         </is>
       </c>
-      <c r="E9" s="3" t="n"/>
-      <c r="F9" s="3" t="inlineStr">
+      <c r="E9" s="12" t="inlineStr">
+        <is>
+          <t>411 - Data Generation</t>
+        </is>
+      </c>
+      <c r="F9" s="12" t="n"/>
+      <c r="G9" s="12" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="G9" s="3" t="n"/>
-      <c r="H9" s="3" t="inlineStr">
+      <c r="H9" s="12" t="n"/>
+      <c r="I9" s="12" t="inlineStr">
         <is>
           <t>2024-07</t>
         </is>
       </c>
-      <c r="I9" s="3" t="n">
+      <c r="J9" s="12" t="n">
         <v>69</v>
       </c>
-      <c r="J9" s="3" t="n">
+      <c r="K9" s="12" t="n">
         <v>69</v>
       </c>
-      <c r="K9" s="1" t="n">
-        <v/>
-      </c>
       <c r="L9" s="1" t="n">
         <v/>
       </c>
@@ -2210,6 +2311,9 @@
         <v/>
       </c>
       <c r="BF9" s="1" t="n">
+        <v/>
+      </c>
+      <c r="BG9" s="1" t="n">
         <v/>
       </c>
     </row>
@@ -2219,34 +2323,36 @@
           <t>Budget</t>
         </is>
       </c>
-      <c r="B10" s="3" t="n"/>
-      <c r="C10" s="3" t="n"/>
-      <c r="D10" s="3" t="inlineStr">
+      <c r="B10" s="12" t="n"/>
+      <c r="C10" s="12" t="n"/>
+      <c r="D10" s="12" t="inlineStr">
         <is>
           <t>T104 - Data Gathering</t>
         </is>
       </c>
-      <c r="E10" s="3" t="n"/>
-      <c r="F10" s="3" t="inlineStr">
+      <c r="E10" s="12" t="inlineStr">
+        <is>
+          <t>411 - Data Generation</t>
+        </is>
+      </c>
+      <c r="F10" s="12" t="n"/>
+      <c r="G10" s="12" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="G10" s="3" t="n"/>
-      <c r="H10" s="3" t="inlineStr">
+      <c r="H10" s="12" t="n"/>
+      <c r="I10" s="12" t="inlineStr">
         <is>
           <t>2024-08</t>
         </is>
       </c>
-      <c r="I10" s="3" t="n">
+      <c r="J10" s="12" t="n">
         <v>63</v>
       </c>
-      <c r="J10" s="3" t="n">
+      <c r="K10" s="12" t="n">
         <v>63</v>
       </c>
-      <c r="K10" s="1" t="n">
-        <v/>
-      </c>
       <c r="L10" s="1" t="n">
         <v/>
       </c>
@@ -2386,6 +2492,9 @@
         <v/>
       </c>
       <c r="BF10" s="1" t="n">
+        <v/>
+      </c>
+      <c r="BG10" s="1" t="n">
         <v/>
       </c>
     </row>
@@ -2395,34 +2504,36 @@
           <t>Budget</t>
         </is>
       </c>
-      <c r="B11" s="3" t="n"/>
-      <c r="C11" s="3" t="n"/>
-      <c r="D11" s="3" t="inlineStr">
+      <c r="B11" s="12" t="n"/>
+      <c r="C11" s="12" t="n"/>
+      <c r="D11" s="12" t="inlineStr">
         <is>
           <t>T104 - Data Gathering</t>
         </is>
       </c>
-      <c r="E11" s="3" t="n"/>
-      <c r="F11" s="3" t="inlineStr">
+      <c r="E11" s="12" t="inlineStr">
+        <is>
+          <t>411 - Data Generation</t>
+        </is>
+      </c>
+      <c r="F11" s="12" t="n"/>
+      <c r="G11" s="12" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="G11" s="3" t="n"/>
-      <c r="H11" s="3" t="inlineStr">
+      <c r="H11" s="12" t="n"/>
+      <c r="I11" s="12" t="inlineStr">
         <is>
           <t>2024-09</t>
         </is>
       </c>
-      <c r="I11" s="3" t="n">
+      <c r="J11" s="12" t="n">
         <v>66</v>
       </c>
-      <c r="J11" s="3" t="n">
+      <c r="K11" s="12" t="n">
         <v>66</v>
       </c>
-      <c r="K11" s="1" t="n">
-        <v/>
-      </c>
       <c r="L11" s="1" t="n">
         <v/>
       </c>
@@ -2562,6 +2673,9 @@
         <v/>
       </c>
       <c r="BF11" s="1" t="n">
+        <v/>
+      </c>
+      <c r="BG11" s="1" t="n">
         <v/>
       </c>
     </row>
@@ -2571,34 +2685,36 @@
           <t>Budget</t>
         </is>
       </c>
-      <c r="B12" s="3" t="n"/>
-      <c r="C12" s="3" t="n"/>
-      <c r="D12" s="3" t="inlineStr">
+      <c r="B12" s="12" t="n"/>
+      <c r="C12" s="12" t="n"/>
+      <c r="D12" s="12" t="inlineStr">
         <is>
           <t>T104 - Data Gathering</t>
         </is>
       </c>
-      <c r="E12" s="3" t="n"/>
-      <c r="F12" s="3" t="inlineStr">
+      <c r="E12" s="12" t="inlineStr">
+        <is>
+          <t>411 - Data Generation</t>
+        </is>
+      </c>
+      <c r="F12" s="12" t="n"/>
+      <c r="G12" s="12" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="G12" s="3" t="n"/>
-      <c r="H12" s="3" t="inlineStr">
+      <c r="H12" s="12" t="n"/>
+      <c r="I12" s="12" t="inlineStr">
         <is>
           <t>2024-10</t>
         </is>
       </c>
-      <c r="I12" s="3" t="n">
+      <c r="J12" s="12" t="n">
         <v>54</v>
       </c>
-      <c r="J12" s="3" t="n">
+      <c r="K12" s="12" t="n">
         <v>54</v>
       </c>
-      <c r="K12" s="1" t="n">
-        <v/>
-      </c>
       <c r="L12" s="1" t="n">
         <v/>
       </c>
@@ -2738,6 +2854,9 @@
         <v/>
       </c>
       <c r="BF12" s="1" t="n">
+        <v/>
+      </c>
+      <c r="BG12" s="1" t="n">
         <v/>
       </c>
     </row>
@@ -2747,34 +2866,36 @@
           <t>Budget</t>
         </is>
       </c>
-      <c r="B13" s="3" t="n"/>
-      <c r="C13" s="3" t="n"/>
-      <c r="D13" s="3" t="inlineStr">
+      <c r="B13" s="12" t="n"/>
+      <c r="C13" s="12" t="n"/>
+      <c r="D13" s="12" t="inlineStr">
         <is>
           <t>T104 - Data Gathering</t>
         </is>
       </c>
-      <c r="E13" s="3" t="n"/>
-      <c r="F13" s="3" t="inlineStr">
+      <c r="E13" s="12" t="inlineStr">
+        <is>
+          <t>411 - Data Generation</t>
+        </is>
+      </c>
+      <c r="F13" s="12" t="n"/>
+      <c r="G13" s="12" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="G13" s="3" t="n"/>
-      <c r="H13" s="3" t="inlineStr">
+      <c r="H13" s="12" t="n"/>
+      <c r="I13" s="12" t="inlineStr">
         <is>
           <t>2024-11</t>
         </is>
       </c>
-      <c r="I13" s="3" t="n">
+      <c r="J13" s="12" t="n">
         <v>60</v>
       </c>
-      <c r="J13" s="3" t="n">
+      <c r="K13" s="12" t="n">
         <v>60</v>
       </c>
-      <c r="K13" s="1" t="n">
-        <v/>
-      </c>
       <c r="L13" s="1" t="n">
         <v/>
       </c>
@@ -2914,6 +3035,9 @@
         <v/>
       </c>
       <c r="BF13" s="1" t="n">
+        <v/>
+      </c>
+      <c r="BG13" s="1" t="n">
         <v/>
       </c>
     </row>
@@ -2923,34 +3047,36 @@
           <t>Budget</t>
         </is>
       </c>
-      <c r="B14" s="3" t="n"/>
-      <c r="C14" s="3" t="n"/>
-      <c r="D14" s="3" t="inlineStr">
+      <c r="B14" s="12" t="n"/>
+      <c r="C14" s="12" t="n"/>
+      <c r="D14" s="12" t="inlineStr">
         <is>
           <t>T104 - Data Gathering</t>
         </is>
       </c>
-      <c r="E14" s="3" t="n"/>
-      <c r="F14" s="3" t="inlineStr">
+      <c r="E14" s="12" t="inlineStr">
+        <is>
+          <t>411 - Data Generation</t>
+        </is>
+      </c>
+      <c r="F14" s="12" t="n"/>
+      <c r="G14" s="12" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="G14" s="3" t="n"/>
-      <c r="H14" s="3" t="inlineStr">
+      <c r="H14" s="12" t="n"/>
+      <c r="I14" s="12" t="inlineStr">
         <is>
           <t>2024-12</t>
         </is>
       </c>
-      <c r="I14" s="3" t="n">
+      <c r="J14" s="12" t="n">
         <v>69</v>
       </c>
-      <c r="J14" s="3" t="n">
+      <c r="K14" s="12" t="n">
         <v>69</v>
       </c>
-      <c r="K14" s="1" t="n">
-        <v/>
-      </c>
       <c r="L14" s="1" t="n">
         <v/>
       </c>
@@ -3090,6 +3216,9 @@
         <v/>
       </c>
       <c r="BF14" s="1" t="n">
+        <v/>
+      </c>
+      <c r="BG14" s="1" t="n">
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
adding colors more accuratly and changed values on the first columns
</commit_message>
<xml_diff>
--- a/data/DataGeneration_5_24.xlsx
+++ b/data/DataGeneration_5_24.xlsx
@@ -50,56 +50,56 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00A2C4C9"/>
-        <bgColor rgb="00A2C4C9"/>
+        <fgColor rgb="001F89DF"/>
+        <bgColor rgb="001F89DF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00F4CCCC"/>
-        <bgColor rgb="00F4CCCC"/>
+        <fgColor rgb="00DF761F"/>
+        <bgColor rgb="00DF761F"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00D3D3D3"/>
-        <bgColor rgb="00D3D3D3"/>
+        <fgColor rgb="00F3C68A"/>
+        <bgColor rgb="00F3C68A"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00F9CB9C"/>
-        <bgColor rgb="00F9CB9C"/>
+        <fgColor rgb="006EEAF3"/>
+        <bgColor rgb="006EEAF3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00D9EAD3"/>
-        <bgColor rgb="00D9EAD3"/>
+        <fgColor rgb="006EF396"/>
+        <bgColor rgb="006EF396"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFF2CC"/>
-        <bgColor rgb="00FFF2CC"/>
+        <fgColor rgb="00E9F483"/>
+        <bgColor rgb="00E9F483"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="009FC5E8"/>
-        <bgColor rgb="009FC5E8"/>
+        <fgColor rgb="004AB3EE"/>
+        <bgColor rgb="004AB3EE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0093C47D"/>
-        <bgColor rgb="0093C47D"/>
+        <fgColor rgb="0055FE33"/>
+        <bgColor rgb="0055FE33"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00EAD1DC"/>
-        <bgColor rgb="00EAD1DC"/>
+        <fgColor rgb="00FC5CE6"/>
+        <bgColor rgb="00FC5CE6"/>
       </patternFill>
     </fill>
   </fills>
@@ -500,7 +500,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BG14"/>
+  <dimension ref="A1:BI14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -575,67 +575,67 @@
           <t>B20/20 - Lavie- Bio.4</t>
         </is>
       </c>
-      <c r="W1" s="4" t="inlineStr">
+      <c r="W1" s="3" t="inlineStr">
         <is>
           <t>B20/20 - Lavie- Bio.5</t>
         </is>
       </c>
-      <c r="X1" s="4" t="inlineStr">
+      <c r="X1" s="3" t="inlineStr">
         <is>
           <t>B20/20 - Lavie- Bio.6</t>
         </is>
       </c>
-      <c r="Y1" s="4" t="inlineStr">
+      <c r="Y1" s="3" t="inlineStr">
         <is>
           <t>B20/20 - Lavie- Bio.7</t>
         </is>
       </c>
-      <c r="Z1" s="4" t="inlineStr">
+      <c r="Z1" s="3" t="inlineStr">
         <is>
           <t>B20/20 - Lavie- Bio.8</t>
         </is>
       </c>
-      <c r="AA1" s="5" t="inlineStr">
+      <c r="AA1" s="4" t="inlineStr">
         <is>
           <t>B40/20 - CPB</t>
         </is>
       </c>
-      <c r="AB1" s="5" t="inlineStr">
+      <c r="AB1" s="4" t="inlineStr">
         <is>
           <t>B40/20 - CPB.1</t>
         </is>
       </c>
-      <c r="AC1" s="5" t="inlineStr">
+      <c r="AC1" s="4" t="inlineStr">
         <is>
           <t>B40/20 - CPB.2</t>
         </is>
       </c>
-      <c r="AD1" s="5" t="inlineStr">
+      <c r="AD1" s="4" t="inlineStr">
         <is>
           <t>B40/20 - CPB.3</t>
         </is>
       </c>
-      <c r="AE1" s="6" t="inlineStr">
+      <c r="AE1" s="5" t="inlineStr">
         <is>
           <t>B70/20 - Biomica</t>
         </is>
       </c>
-      <c r="AF1" s="6" t="inlineStr">
+      <c r="AF1" s="5" t="inlineStr">
         <is>
           <t>B70/20 - Biomica.1</t>
         </is>
       </c>
-      <c r="AG1" s="6" t="inlineStr">
+      <c r="AG1" s="5" t="inlineStr">
         <is>
           <t>B70/20 - Biomica.2</t>
         </is>
       </c>
-      <c r="AH1" s="6" t="inlineStr">
+      <c r="AH1" s="5" t="inlineStr">
         <is>
           <t>B70/20 - Biomica.3</t>
         </is>
       </c>
-      <c r="AI1" s="6" t="inlineStr">
+      <c r="AI1" s="5" t="inlineStr">
         <is>
           <t>B70/20 - Biomica.4</t>
         </is>
@@ -645,113 +645,115 @@
           <t>B74/20 - Canonic</t>
         </is>
       </c>
-      <c r="AK1" s="7" t="inlineStr">
+      <c r="AK1" s="6" t="inlineStr">
         <is>
           <t>B74/20 - Canonic.1</t>
         </is>
       </c>
-      <c r="AL1" s="7" t="inlineStr">
+      <c r="AL1" s="6" t="inlineStr">
         <is>
           <t>B74/20 - Canonic.2</t>
         </is>
       </c>
-      <c r="AM1" s="7" t="inlineStr">
+      <c r="AM1" s="6" t="inlineStr">
         <is>
           <t>B74/20 - Canonic.3</t>
         </is>
       </c>
-      <c r="AN1" s="7" t="inlineStr">
+      <c r="AN1" s="6" t="inlineStr">
         <is>
           <t>B74/20 - Canonic.4</t>
         </is>
       </c>
-      <c r="AO1" s="7" t="inlineStr">
+      <c r="AO1" s="6" t="inlineStr">
         <is>
           <t>B74/20 - Canonic.5</t>
         </is>
       </c>
-      <c r="AP1" s="8" t="inlineStr">
+      <c r="AP1" s="7" t="inlineStr">
         <is>
           <t>B80/20 - PRoduct</t>
         </is>
       </c>
-      <c r="AQ1" s="8" t="inlineStr">
+      <c r="AQ1" s="7" t="inlineStr">
         <is>
           <t>B80/20 - PRoduct.1</t>
         </is>
       </c>
-      <c r="AR1" s="8" t="inlineStr">
+      <c r="AR1" s="7" t="inlineStr">
         <is>
           <t>B80/20 - PRoduct.2</t>
         </is>
       </c>
-      <c r="AS1" s="8" t="inlineStr">
+      <c r="AS1" s="7" t="inlineStr">
         <is>
           <t>B80/20 - PRoduct.3</t>
         </is>
       </c>
-      <c r="AT1" s="8" t="inlineStr">
+      <c r="AT1" s="7" t="inlineStr">
         <is>
           <t>B80/20 - PRoduct.4</t>
         </is>
       </c>
-      <c r="AU1" s="8" t="inlineStr">
+      <c r="AU1" s="7" t="inlineStr">
         <is>
           <t>B80/20 - PRoduct.5</t>
         </is>
       </c>
-      <c r="AV1" s="8" t="inlineStr">
+      <c r="AV1" s="7" t="inlineStr">
         <is>
           <t>B80/20 - PRoduct.6</t>
         </is>
       </c>
-      <c r="AW1" s="8" t="inlineStr">
+      <c r="AW1" s="7" t="inlineStr">
         <is>
           <t>B80/20 - PRoduct.7</t>
         </is>
       </c>
-      <c r="AX1" s="8" t="inlineStr">
+      <c r="AX1" s="7" t="inlineStr">
         <is>
           <t>B80/20 - PRoduct.8</t>
         </is>
       </c>
-      <c r="AY1" s="8" t="inlineStr">
+      <c r="AY1" s="7" t="inlineStr">
         <is>
           <t>B80/20 - PRoduct.9</t>
         </is>
       </c>
-      <c r="AZ1" s="9" t="inlineStr">
+      <c r="AZ1" s="8" t="inlineStr">
         <is>
           <t>B72/20 - Casterra</t>
         </is>
       </c>
-      <c r="BA1" s="9" t="inlineStr">
+      <c r="BA1" s="8" t="inlineStr">
         <is>
           <t>B72/20 - Casterra.1</t>
         </is>
       </c>
-      <c r="BB1" s="9" t="inlineStr">
+      <c r="BB1" s="8" t="inlineStr">
         <is>
           <t>B72/20 - Casterra.2</t>
         </is>
       </c>
-      <c r="BC1" s="9" t="inlineStr">
+      <c r="BC1" s="8" t="inlineStr">
         <is>
           <t>B72/20 - Casterra.3</t>
         </is>
       </c>
-      <c r="BD1" s="9" t="inlineStr">
+      <c r="BD1" s="8" t="inlineStr">
         <is>
           <t>B72/20 - Casterra.4</t>
         </is>
       </c>
-      <c r="BE1" s="9" t="inlineStr">
+      <c r="BE1" s="8" t="inlineStr">
         <is>
           <t>B72/20 - Casterra.5</t>
         </is>
       </c>
-      <c r="BF1" s="10" t="n"/>
+      <c r="BF1" s="9" t="n"/>
       <c r="BG1" s="10" t="n"/>
+      <c r="BH1" s="1" t="n"/>
+      <c r="BI1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="11" t="inlineStr">
@@ -1049,15 +1051,29 @@
           <t>P0 - Vacation / Sickness</t>
         </is>
       </c>
+      <c r="BH2" s="11" t="inlineStr">
+        <is>
+          <t>New project1</t>
+        </is>
+      </c>
+      <c r="BI2" s="11" t="inlineStr">
+        <is>
+          <t>New project2</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Budget</t>
+          <t>ACTUAL</t>
         </is>
       </c>
       <c r="B3" s="12" t="n"/>
-      <c r="C3" s="12" t="n"/>
+      <c r="C3" s="12" t="inlineStr">
+        <is>
+          <t>Ongoing task</t>
+        </is>
+      </c>
       <c r="D3" s="12" t="inlineStr">
         <is>
           <t>T104 - Data Gathering</t>
@@ -1230,15 +1246,21 @@
       <c r="BG3" s="1" t="n">
         <v/>
       </c>
+      <c r="BH3" s="1" t="n"/>
+      <c r="BI3" s="1" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Budget</t>
+          <t>ACTUAL</t>
         </is>
       </c>
       <c r="B4" s="12" t="n"/>
-      <c r="C4" s="12" t="n"/>
+      <c r="C4" s="12" t="inlineStr">
+        <is>
+          <t>Ongoing task</t>
+        </is>
+      </c>
       <c r="D4" s="12" t="inlineStr">
         <is>
           <t>T104 - Data Gathering</t>
@@ -1411,15 +1433,21 @@
       <c r="BG4" s="1" t="n">
         <v/>
       </c>
+      <c r="BH4" s="1" t="n"/>
+      <c r="BI4" s="1" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Budget</t>
+          <t>ACTUAL</t>
         </is>
       </c>
       <c r="B5" s="12" t="n"/>
-      <c r="C5" s="12" t="n"/>
+      <c r="C5" s="12" t="inlineStr">
+        <is>
+          <t>Ongoing task</t>
+        </is>
+      </c>
       <c r="D5" s="12" t="inlineStr">
         <is>
           <t>T104 - Data Gathering</t>
@@ -1592,15 +1620,21 @@
       <c r="BG5" s="1" t="n">
         <v>11</v>
       </c>
+      <c r="BH5" s="1" t="n"/>
+      <c r="BI5" s="1" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Budget</t>
+          <t>ACTUAL</t>
         </is>
       </c>
       <c r="B6" s="12" t="n"/>
-      <c r="C6" s="12" t="n"/>
+      <c r="C6" s="12" t="inlineStr">
+        <is>
+          <t>Ongoing task</t>
+        </is>
+      </c>
       <c r="D6" s="12" t="inlineStr">
         <is>
           <t>T104 - Data Gathering</t>
@@ -1773,15 +1807,21 @@
       <c r="BG6" s="1" t="n">
         <v/>
       </c>
+      <c r="BH6" s="1" t="n"/>
+      <c r="BI6" s="1" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Budget</t>
+          <t>ACTUAL</t>
         </is>
       </c>
       <c r="B7" s="12" t="n"/>
-      <c r="C7" s="12" t="n"/>
+      <c r="C7" s="12" t="inlineStr">
+        <is>
+          <t>Ongoing task</t>
+        </is>
+      </c>
       <c r="D7" s="12" t="inlineStr">
         <is>
           <t>T104 - Data Gathering</t>
@@ -1954,15 +1994,21 @@
       <c r="BG7" s="1" t="n">
         <v/>
       </c>
+      <c r="BH7" s="1" t="n"/>
+      <c r="BI7" s="1" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Budget</t>
+          <t>ACTUAL</t>
         </is>
       </c>
       <c r="B8" s="12" t="n"/>
-      <c r="C8" s="12" t="n"/>
+      <c r="C8" s="12" t="inlineStr">
+        <is>
+          <t>Ongoing task</t>
+        </is>
+      </c>
       <c r="D8" s="12" t="inlineStr">
         <is>
           <t>T104 - Data Gathering</t>
@@ -2135,15 +2181,21 @@
       <c r="BG8" s="1" t="n">
         <v/>
       </c>
+      <c r="BH8" s="1" t="n"/>
+      <c r="BI8" s="1" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Budget</t>
+          <t>ACTUAL</t>
         </is>
       </c>
       <c r="B9" s="12" t="n"/>
-      <c r="C9" s="12" t="n"/>
+      <c r="C9" s="12" t="inlineStr">
+        <is>
+          <t>Ongoing task</t>
+        </is>
+      </c>
       <c r="D9" s="12" t="inlineStr">
         <is>
           <t>T104 - Data Gathering</t>
@@ -2316,15 +2368,21 @@
       <c r="BG9" s="1" t="n">
         <v/>
       </c>
+      <c r="BH9" s="1" t="n"/>
+      <c r="BI9" s="1" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Budget</t>
+          <t>ACTUAL</t>
         </is>
       </c>
       <c r="B10" s="12" t="n"/>
-      <c r="C10" s="12" t="n"/>
+      <c r="C10" s="12" t="inlineStr">
+        <is>
+          <t>Ongoing task</t>
+        </is>
+      </c>
       <c r="D10" s="12" t="inlineStr">
         <is>
           <t>T104 - Data Gathering</t>
@@ -2497,15 +2555,21 @@
       <c r="BG10" s="1" t="n">
         <v/>
       </c>
+      <c r="BH10" s="1" t="n"/>
+      <c r="BI10" s="1" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Budget</t>
+          <t>ACTUAL</t>
         </is>
       </c>
       <c r="B11" s="12" t="n"/>
-      <c r="C11" s="12" t="n"/>
+      <c r="C11" s="12" t="inlineStr">
+        <is>
+          <t>Ongoing task</t>
+        </is>
+      </c>
       <c r="D11" s="12" t="inlineStr">
         <is>
           <t>T104 - Data Gathering</t>
@@ -2678,15 +2742,21 @@
       <c r="BG11" s="1" t="n">
         <v/>
       </c>
+      <c r="BH11" s="1" t="n"/>
+      <c r="BI11" s="1" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Budget</t>
+          <t>ACTUAL</t>
         </is>
       </c>
       <c r="B12" s="12" t="n"/>
-      <c r="C12" s="12" t="n"/>
+      <c r="C12" s="12" t="inlineStr">
+        <is>
+          <t>Ongoing task</t>
+        </is>
+      </c>
       <c r="D12" s="12" t="inlineStr">
         <is>
           <t>T104 - Data Gathering</t>
@@ -2859,15 +2929,21 @@
       <c r="BG12" s="1" t="n">
         <v/>
       </c>
+      <c r="BH12" s="1" t="n"/>
+      <c r="BI12" s="1" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Budget</t>
+          <t>ACTUAL</t>
         </is>
       </c>
       <c r="B13" s="12" t="n"/>
-      <c r="C13" s="12" t="n"/>
+      <c r="C13" s="12" t="inlineStr">
+        <is>
+          <t>Ongoing task</t>
+        </is>
+      </c>
       <c r="D13" s="12" t="inlineStr">
         <is>
           <t>T104 - Data Gathering</t>
@@ -3040,15 +3116,21 @@
       <c r="BG13" s="1" t="n">
         <v/>
       </c>
+      <c r="BH13" s="1" t="n"/>
+      <c r="BI13" s="1" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Budget</t>
+          <t>ACTUAL</t>
         </is>
       </c>
       <c r="B14" s="12" t="n"/>
-      <c r="C14" s="12" t="n"/>
+      <c r="C14" s="12" t="inlineStr">
+        <is>
+          <t>Ongoing task</t>
+        </is>
+      </c>
       <c r="D14" s="12" t="inlineStr">
         <is>
           <t>T104 - Data Gathering</t>
@@ -3221,6 +3303,8 @@
       <c r="BG14" s="1" t="n">
         <v/>
       </c>
+      <c r="BH14" s="1" t="n"/>
+      <c r="BI14" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fixing bugs in data place for page 2 in excel input
</commit_message>
<xml_diff>
--- a/data/DataGeneration_5_24.xlsx
+++ b/data/DataGeneration_5_24.xlsx
@@ -1053,12 +1053,12 @@
       </c>
       <c r="BH2" s="11" t="inlineStr">
         <is>
-          <t>New project1</t>
+          <t>New Project 1</t>
         </is>
       </c>
       <c r="BI2" s="11" t="inlineStr">
         <is>
-          <t>New project2</t>
+          <t>New Project 2</t>
         </is>
       </c>
     </row>
@@ -1474,10 +1474,10 @@
         <v>63</v>
       </c>
       <c r="K5" s="12" t="n">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="L5" s="1" t="n">
-        <v>4</v>
+        <v/>
       </c>
       <c r="M5" s="1" t="n">
         <v/>
@@ -1495,7 +1495,7 @@
         <v/>
       </c>
       <c r="R5" s="1" t="n">
-        <v>4</v>
+        <v/>
       </c>
       <c r="S5" s="1" t="n">
         <v/>
@@ -1507,7 +1507,7 @@
         <v/>
       </c>
       <c r="V5" s="1" t="n">
-        <v>16</v>
+        <v/>
       </c>
       <c r="W5" s="1" t="n">
         <v/>
@@ -1525,13 +1525,13 @@
         <v/>
       </c>
       <c r="AB5" s="1" t="n">
-        <v>4</v>
+        <v/>
       </c>
       <c r="AC5" s="1" t="n">
         <v/>
       </c>
       <c r="AD5" s="1" t="n">
-        <v>4</v>
+        <v/>
       </c>
       <c r="AE5" s="1" t="n">
         <v/>
@@ -1561,7 +1561,7 @@
         <v/>
       </c>
       <c r="AN5" s="1" t="n">
-        <v>5</v>
+        <v/>
       </c>
       <c r="AO5" s="1" t="n">
         <v/>
@@ -1591,7 +1591,7 @@
         <v/>
       </c>
       <c r="AX5" s="1" t="n">
-        <v>4</v>
+        <v/>
       </c>
       <c r="AY5" s="1" t="n">
         <v/>
@@ -1606,7 +1606,7 @@
         <v/>
       </c>
       <c r="BC5" s="1" t="n">
-        <v>6.8</v>
+        <v/>
       </c>
       <c r="BD5" s="1" t="n">
         <v/>
@@ -1615,10 +1615,10 @@
         <v/>
       </c>
       <c r="BF5" s="1" t="n">
-        <v>4.2</v>
+        <v/>
       </c>
       <c r="BG5" s="1" t="n">
-        <v>11</v>
+        <v/>
       </c>
       <c r="BH5" s="1" t="n"/>
       <c r="BI5" s="1" t="n"/>

</xml_diff>